<commit_message>
sn: tas1 may 2021 add form for senegal.
</commit_message>
<xml_diff>
--- a/LF/TAS/Senegal/TAS1/Mai 2021/sn_lf_tas1_2_partcipants_202105.xlsx
+++ b/LF/TAS/Senegal/TAS1/Mai 2021/sn_lf_tas1_2_partcipants_202105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Senegal\TAS2\Avr 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Senegal\TAS1\Mai 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6D776F-9CB8-4755-A3E2-4CEBA64A275A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B8F88-421E-49E2-8967-0B6A0C12BE33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -356,10 +356,10 @@
     <t>Sélectionner votre commune</t>
   </si>
   <si>
-    <t>sn_lf_tas1_2_partcipants_202104_v2</t>
-  </si>
-  <si>
-    <t>(Avril 2021) 2. TAS1 FL - Formulaire Participants V2</t>
+    <t>(Mai 2021) 2. TAS1 FL - Formulaire Participants</t>
+  </si>
+  <si>
+    <t>sn_lf_tas1_2_partcipants_202105</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1554,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>109</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
       </c>
       <c r="C2">
         <v>20210419</v>

</xml_diff>